<commit_message>
Tried something don't think it worked
</commit_message>
<xml_diff>
--- a/plant_input_1_cut.xlsx
+++ b/plant_input_1_cut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Farm-Squire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39F8A0E-6DAC-434D-AE2F-884BF5DED2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A330BB11-7679-414B-BB5D-C8FD7E176166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4785" windowWidth="29040" windowHeight="15720" tabRatio="574" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,10 +589,10 @@
   <dimension ref="A1:AA985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -774,25 +774,25 @@
         <v>26</v>
       </c>
       <c r="C3" s="3">
-        <v>3.1776470589999999</v>
+        <v>3.8099908142267198</v>
       </c>
       <c r="D3" s="3">
-        <v>12.71058824</v>
+        <v>15.239963256906879</v>
       </c>
       <c r="E3" s="3">
-        <v>11.121764710000001</v>
+        <v>13.334967849793516</v>
       </c>
       <c r="F3" s="3">
-        <v>3.8527568919999999</v>
+        <v>5.0442037993743662</v>
       </c>
       <c r="G3" s="3">
-        <v>3.297243108</v>
+        <v>4.3155965839091799</v>
       </c>
       <c r="H3" s="3">
-        <v>3.6434891110000001</v>
+        <v>6.5803022134931641</v>
       </c>
       <c r="I3" s="3">
-        <v>3.8265108890000001</v>
+        <v>6.9093173241678212</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -801,16 +801,16 @@
         <v>0</v>
       </c>
       <c r="L3" s="3">
-        <v>9.4363870970000008</v>
+        <v>1.1975759651113547</v>
       </c>
       <c r="M3" s="3">
-        <v>1.8023906350000001</v>
+        <v>0.77842437732238057</v>
       </c>
       <c r="N3" s="3">
-        <v>8.8733774830000005</v>
+        <v>8.2397552479535676</v>
       </c>
       <c r="O3" s="3">
-        <v>14.496622520000001</v>
+        <v>13.458266904990829</v>
       </c>
       <c r="P3" s="3">
         <v>0</v>
@@ -831,10 +831,10 @@
         <v>0</v>
       </c>
       <c r="V3" s="3">
-        <v>11.434862109999999</v>
+        <v>12.406844507500125</v>
       </c>
       <c r="W3" s="3">
-        <v>8.0051378920000005</v>
+        <v>8.6847911552500872</v>
       </c>
       <c r="X3" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
dry matter yield per hectare has been changed
</commit_message>
<xml_diff>
--- a/plant_input_1_cut.xlsx
+++ b/plant_input_1_cut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Farm-Squire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A330BB11-7679-414B-BB5D-C8FD7E176166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C68EAD4-A0B0-47FA-8D22-61A8944D6AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4785" windowWidth="29040" windowHeight="15720" tabRatio="574" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,10 +589,10 @@
   <dimension ref="A1:AA985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
+      <selection pane="bottomRight" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1770,25 +1770,25 @@
         <v>41</v>
       </c>
       <c r="C15" s="3">
-        <v>3123.0169507616724</v>
+        <v>2924</v>
       </c>
       <c r="D15" s="3">
-        <v>12492.067806977921</v>
+        <v>2924</v>
       </c>
       <c r="E15" s="3">
-        <v>10930.559331105682</v>
+        <v>2924</v>
       </c>
       <c r="F15" s="3">
-        <v>1002.6260425465119</v>
+        <v>3191.5555555555547</v>
       </c>
       <c r="G15" s="3">
-        <v>858.06135745348809</v>
+        <v>3191.5555555555547</v>
       </c>
       <c r="H15" s="3">
-        <v>1236.9099008478349</v>
+        <v>4407.5</v>
       </c>
       <c r="I15" s="3">
-        <v>1299.0430491521652</v>
+        <v>4407.5</v>
       </c>
       <c r="J15" s="3">
         <v>1104</v>
@@ -1797,16 +1797,16 @@
         <v>1435</v>
       </c>
       <c r="L15" s="3">
-        <v>2429.2506504839375</v>
+        <v>309.67200000000003</v>
       </c>
       <c r="M15" s="3">
-        <v>463.99735168684407</v>
+        <v>309.67200000000003</v>
       </c>
       <c r="N15" s="3">
-        <v>3772.0550212683343</v>
+        <v>2264.666666666667</v>
       </c>
       <c r="O15" s="3">
-        <v>6162.4852400069612</v>
+        <v>2264.666666666667</v>
       </c>
       <c r="P15" s="3">
         <f>(P2/100)*(478771.7688+46926)</f>
@@ -1831,10 +1831,10 @@
         <v>3534</v>
       </c>
       <c r="V15" s="3">
-        <v>7319.2574134964962</v>
+        <v>2264.666666666667</v>
       </c>
       <c r="W15" s="3">
-        <v>5123.9502757836681</v>
+        <v>2264.666666666667</v>
       </c>
       <c r="X15" s="3">
         <v>1958.65</v>

</xml_diff>